<commit_message>
Corrección AC, PV y EV de CI4
</commit_message>
<xml_diff>
--- a/Planificación del proyecto/CI4 Equipo 01.xlsx
+++ b/Planificación del proyecto/CI4 Equipo 01.xlsx
@@ -5,7 +5,7 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\franc\OneDrive\Desktop\New folder (5)\Ecommerce-Sports\Planificación del proyecto\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\MeDicenTecno\Desktop\PS\Ecommerce-Sports\Planificación del proyecto\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -23,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1620" uniqueCount="292">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1589" uniqueCount="293">
   <si>
     <t>Nro Hito</t>
   </si>
@@ -898,7 +898,10 @@
     <t>9hs.</t>
   </si>
   <si>
-    <t>ABMs carrito y producto</t>
+    <t>3; 9</t>
+  </si>
+  <si>
+    <t>3; 49</t>
   </si>
 </sst>
 </file>
@@ -1364,23 +1367,29 @@
       <alignment horizontal="center" vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -1396,12 +1405,6 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -5748,91 +5751,91 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:37" x14ac:dyDescent="0.2">
-      <c r="A1" s="73" t="s">
+      <c r="A1" s="76" t="s">
         <v>26</v>
       </c>
-      <c r="B1" s="76" t="s">
+      <c r="B1" s="80" t="s">
         <v>27</v>
       </c>
-      <c r="C1" s="77"/>
-      <c r="D1" s="73" t="s">
+      <c r="C1" s="81"/>
+      <c r="D1" s="76" t="s">
         <v>28</v>
       </c>
-      <c r="E1" s="73" t="s">
+      <c r="E1" s="76" t="s">
         <v>3</v>
       </c>
-      <c r="F1" s="73" t="s">
+      <c r="F1" s="76" t="s">
         <v>29</v>
       </c>
-      <c r="G1" s="73" t="s">
+      <c r="G1" s="76" t="s">
         <v>30</v>
       </c>
-      <c r="H1" s="73" t="s">
+      <c r="H1" s="76" t="s">
         <v>31</v>
       </c>
-      <c r="I1" s="73" t="s">
+      <c r="I1" s="76" t="s">
         <v>32</v>
       </c>
-      <c r="J1" s="73" t="s">
+      <c r="J1" s="76" t="s">
         <v>33</v>
       </c>
-      <c r="K1" s="83" t="s">
+      <c r="K1" s="73" t="s">
         <v>34</v>
       </c>
-      <c r="L1" s="81"/>
-      <c r="M1" s="82"/>
-      <c r="N1" s="80" t="s">
+      <c r="L1" s="74"/>
+      <c r="M1" s="75"/>
+      <c r="N1" s="79" t="s">
         <v>35</v>
       </c>
-      <c r="O1" s="81"/>
-      <c r="P1" s="82"/>
-      <c r="Q1" s="83" t="s">
+      <c r="O1" s="74"/>
+      <c r="P1" s="75"/>
+      <c r="Q1" s="73" t="s">
         <v>8</v>
       </c>
-      <c r="R1" s="81"/>
-      <c r="S1" s="82"/>
-      <c r="T1" s="80" t="s">
+      <c r="R1" s="74"/>
+      <c r="S1" s="75"/>
+      <c r="T1" s="79" t="s">
         <v>9</v>
       </c>
-      <c r="U1" s="81"/>
-      <c r="V1" s="82"/>
-      <c r="W1" s="83" t="s">
+      <c r="U1" s="74"/>
+      <c r="V1" s="75"/>
+      <c r="W1" s="73" t="s">
         <v>10</v>
       </c>
-      <c r="X1" s="81"/>
-      <c r="Y1" s="82"/>
-      <c r="Z1" s="80" t="s">
+      <c r="X1" s="74"/>
+      <c r="Y1" s="75"/>
+      <c r="Z1" s="79" t="s">
         <v>11</v>
       </c>
-      <c r="AA1" s="81"/>
-      <c r="AB1" s="82"/>
-      <c r="AC1" s="83" t="s">
+      <c r="AA1" s="74"/>
+      <c r="AB1" s="75"/>
+      <c r="AC1" s="73" t="s">
         <v>12</v>
       </c>
-      <c r="AD1" s="81"/>
-      <c r="AE1" s="82"/>
-      <c r="AF1" s="80" t="s">
+      <c r="AD1" s="74"/>
+      <c r="AE1" s="75"/>
+      <c r="AF1" s="79" t="s">
         <v>13</v>
       </c>
-      <c r="AG1" s="81"/>
-      <c r="AH1" s="82"/>
-      <c r="AI1" s="83" t="s">
+      <c r="AG1" s="74"/>
+      <c r="AH1" s="75"/>
+      <c r="AI1" s="73" t="s">
         <v>14</v>
       </c>
-      <c r="AJ1" s="81"/>
-      <c r="AK1" s="82"/>
+      <c r="AJ1" s="74"/>
+      <c r="AK1" s="75"/>
     </row>
     <row r="2" spans="1:37" x14ac:dyDescent="0.2">
-      <c r="A2" s="74"/>
-      <c r="B2" s="78"/>
-      <c r="C2" s="79"/>
-      <c r="D2" s="74"/>
-      <c r="E2" s="74"/>
-      <c r="F2" s="74"/>
-      <c r="G2" s="74"/>
-      <c r="H2" s="74"/>
-      <c r="I2" s="74"/>
-      <c r="J2" s="74"/>
+      <c r="A2" s="77"/>
+      <c r="B2" s="82"/>
+      <c r="C2" s="83"/>
+      <c r="D2" s="77"/>
+      <c r="E2" s="77"/>
+      <c r="F2" s="77"/>
+      <c r="G2" s="77"/>
+      <c r="H2" s="77"/>
+      <c r="I2" s="77"/>
+      <c r="J2" s="77"/>
       <c r="K2" s="3">
         <v>44081</v>
       </c>
@@ -5915,20 +5918,20 @@
       </c>
     </row>
     <row r="3" spans="1:37" x14ac:dyDescent="0.2">
-      <c r="A3" s="75"/>
+      <c r="A3" s="78"/>
       <c r="B3" s="8" t="s">
         <v>15</v>
       </c>
       <c r="C3" s="8" t="s">
         <v>16</v>
       </c>
-      <c r="D3" s="75"/>
-      <c r="E3" s="75"/>
-      <c r="F3" s="75"/>
-      <c r="G3" s="75"/>
-      <c r="H3" s="75"/>
-      <c r="I3" s="75"/>
-      <c r="J3" s="75"/>
+      <c r="D3" s="78"/>
+      <c r="E3" s="78"/>
+      <c r="F3" s="78"/>
+      <c r="G3" s="78"/>
+      <c r="H3" s="78"/>
+      <c r="I3" s="78"/>
+      <c r="J3" s="78"/>
       <c r="K3" s="9" t="s">
         <v>36</v>
       </c>
@@ -35954,6 +35957,16 @@
     </row>
   </sheetData>
   <mergeCells count="18">
+    <mergeCell ref="A1:A3"/>
+    <mergeCell ref="B1:C2"/>
+    <mergeCell ref="D1:D3"/>
+    <mergeCell ref="E1:E3"/>
+    <mergeCell ref="F1:F3"/>
+    <mergeCell ref="G1:G3"/>
+    <mergeCell ref="H1:H3"/>
+    <mergeCell ref="Z1:AB1"/>
+    <mergeCell ref="AC1:AE1"/>
+    <mergeCell ref="AF1:AH1"/>
     <mergeCell ref="AI1:AK1"/>
     <mergeCell ref="I1:I3"/>
     <mergeCell ref="J1:J3"/>
@@ -35962,16 +35975,6 @@
     <mergeCell ref="Q1:S1"/>
     <mergeCell ref="T1:V1"/>
     <mergeCell ref="W1:Y1"/>
-    <mergeCell ref="G1:G3"/>
-    <mergeCell ref="H1:H3"/>
-    <mergeCell ref="Z1:AB1"/>
-    <mergeCell ref="AC1:AE1"/>
-    <mergeCell ref="AF1:AH1"/>
-    <mergeCell ref="A1:A3"/>
-    <mergeCell ref="B1:C2"/>
-    <mergeCell ref="D1:D3"/>
-    <mergeCell ref="E1:E3"/>
-    <mergeCell ref="F1:F3"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="360" verticalDpi="360" r:id="rId1"/>
@@ -35996,91 +35999,91 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:37" x14ac:dyDescent="0.2">
-      <c r="A1" s="73" t="s">
+      <c r="A1" s="76" t="s">
         <v>26</v>
       </c>
-      <c r="B1" s="76" t="s">
+      <c r="B1" s="80" t="s">
         <v>27</v>
       </c>
-      <c r="C1" s="77"/>
-      <c r="D1" s="73" t="s">
+      <c r="C1" s="81"/>
+      <c r="D1" s="76" t="s">
         <v>28</v>
       </c>
-      <c r="E1" s="73" t="s">
+      <c r="E1" s="76" t="s">
         <v>3</v>
       </c>
-      <c r="F1" s="73" t="s">
+      <c r="F1" s="76" t="s">
         <v>29</v>
       </c>
-      <c r="G1" s="73" t="s">
+      <c r="G1" s="76" t="s">
         <v>30</v>
       </c>
-      <c r="H1" s="73" t="s">
+      <c r="H1" s="76" t="s">
         <v>31</v>
       </c>
-      <c r="I1" s="73" t="s">
+      <c r="I1" s="76" t="s">
         <v>32</v>
       </c>
-      <c r="J1" s="73" t="s">
+      <c r="J1" s="76" t="s">
         <v>33</v>
       </c>
-      <c r="K1" s="83" t="s">
+      <c r="K1" s="73" t="s">
         <v>34</v>
       </c>
-      <c r="L1" s="81"/>
-      <c r="M1" s="82"/>
-      <c r="N1" s="80" t="s">
+      <c r="L1" s="74"/>
+      <c r="M1" s="75"/>
+      <c r="N1" s="79" t="s">
         <v>35</v>
       </c>
-      <c r="O1" s="81"/>
-      <c r="P1" s="82"/>
-      <c r="Q1" s="83" t="s">
+      <c r="O1" s="74"/>
+      <c r="P1" s="75"/>
+      <c r="Q1" s="73" t="s">
         <v>8</v>
       </c>
-      <c r="R1" s="81"/>
-      <c r="S1" s="82"/>
-      <c r="T1" s="80" t="s">
+      <c r="R1" s="74"/>
+      <c r="S1" s="75"/>
+      <c r="T1" s="79" t="s">
         <v>9</v>
       </c>
-      <c r="U1" s="81"/>
-      <c r="V1" s="82"/>
-      <c r="W1" s="83" t="s">
+      <c r="U1" s="74"/>
+      <c r="V1" s="75"/>
+      <c r="W1" s="73" t="s">
         <v>10</v>
       </c>
-      <c r="X1" s="81"/>
-      <c r="Y1" s="82"/>
-      <c r="Z1" s="80" t="s">
+      <c r="X1" s="74"/>
+      <c r="Y1" s="75"/>
+      <c r="Z1" s="79" t="s">
         <v>11</v>
       </c>
-      <c r="AA1" s="81"/>
-      <c r="AB1" s="82"/>
-      <c r="AC1" s="83" t="s">
+      <c r="AA1" s="74"/>
+      <c r="AB1" s="75"/>
+      <c r="AC1" s="73" t="s">
         <v>12</v>
       </c>
-      <c r="AD1" s="81"/>
-      <c r="AE1" s="82"/>
-      <c r="AF1" s="80" t="s">
+      <c r="AD1" s="74"/>
+      <c r="AE1" s="75"/>
+      <c r="AF1" s="79" t="s">
         <v>13</v>
       </c>
-      <c r="AG1" s="81"/>
-      <c r="AH1" s="82"/>
-      <c r="AI1" s="83" t="s">
+      <c r="AG1" s="74"/>
+      <c r="AH1" s="75"/>
+      <c r="AI1" s="73" t="s">
         <v>14</v>
       </c>
-      <c r="AJ1" s="81"/>
-      <c r="AK1" s="82"/>
+      <c r="AJ1" s="74"/>
+      <c r="AK1" s="75"/>
     </row>
     <row r="2" spans="1:37" x14ac:dyDescent="0.2">
-      <c r="A2" s="74"/>
-      <c r="B2" s="78"/>
-      <c r="C2" s="79"/>
-      <c r="D2" s="74"/>
-      <c r="E2" s="74"/>
-      <c r="F2" s="74"/>
-      <c r="G2" s="74"/>
-      <c r="H2" s="74"/>
-      <c r="I2" s="74"/>
-      <c r="J2" s="74"/>
+      <c r="A2" s="77"/>
+      <c r="B2" s="82"/>
+      <c r="C2" s="83"/>
+      <c r="D2" s="77"/>
+      <c r="E2" s="77"/>
+      <c r="F2" s="77"/>
+      <c r="G2" s="77"/>
+      <c r="H2" s="77"/>
+      <c r="I2" s="77"/>
+      <c r="J2" s="77"/>
       <c r="K2" s="3">
         <v>44081</v>
       </c>
@@ -36163,20 +36166,20 @@
       </c>
     </row>
     <row r="3" spans="1:37" x14ac:dyDescent="0.2">
-      <c r="A3" s="75"/>
+      <c r="A3" s="78"/>
       <c r="B3" s="8" t="s">
         <v>15</v>
       </c>
       <c r="C3" s="8" t="s">
         <v>16</v>
       </c>
-      <c r="D3" s="75"/>
-      <c r="E3" s="75"/>
-      <c r="F3" s="75"/>
-      <c r="G3" s="75"/>
-      <c r="H3" s="75"/>
-      <c r="I3" s="75"/>
-      <c r="J3" s="75"/>
+      <c r="D3" s="78"/>
+      <c r="E3" s="78"/>
+      <c r="F3" s="78"/>
+      <c r="G3" s="78"/>
+      <c r="H3" s="78"/>
+      <c r="I3" s="78"/>
+      <c r="J3" s="78"/>
       <c r="K3" s="9" t="s">
         <v>36</v>
       </c>
@@ -38654,6 +38657,12 @@
     </row>
   </sheetData>
   <mergeCells count="18">
+    <mergeCell ref="G1:G3"/>
+    <mergeCell ref="A1:A3"/>
+    <mergeCell ref="B1:C2"/>
+    <mergeCell ref="D1:D3"/>
+    <mergeCell ref="E1:E3"/>
+    <mergeCell ref="F1:F3"/>
     <mergeCell ref="AI1:AK1"/>
     <mergeCell ref="H1:H3"/>
     <mergeCell ref="I1:I3"/>
@@ -38666,12 +38675,6 @@
     <mergeCell ref="Z1:AB1"/>
     <mergeCell ref="AC1:AE1"/>
     <mergeCell ref="AF1:AH1"/>
-    <mergeCell ref="G1:G3"/>
-    <mergeCell ref="A1:A3"/>
-    <mergeCell ref="B1:C2"/>
-    <mergeCell ref="D1:D3"/>
-    <mergeCell ref="E1:E3"/>
-    <mergeCell ref="F1:F3"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -38695,79 +38698,79 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:45" x14ac:dyDescent="0.2">
-      <c r="A1" s="73" t="s">
+      <c r="A1" s="76" t="s">
         <v>26</v>
       </c>
-      <c r="B1" s="76" t="s">
+      <c r="B1" s="80" t="s">
         <v>27</v>
       </c>
-      <c r="C1" s="86"/>
-      <c r="D1" s="73" t="s">
+      <c r="C1" s="88"/>
+      <c r="D1" s="76" t="s">
         <v>28</v>
       </c>
-      <c r="E1" s="73" t="s">
+      <c r="E1" s="76" t="s">
         <v>3</v>
       </c>
-      <c r="F1" s="73" t="s">
+      <c r="F1" s="76" t="s">
         <v>29</v>
       </c>
-      <c r="G1" s="73" t="s">
+      <c r="G1" s="76" t="s">
         <v>30</v>
       </c>
-      <c r="H1" s="73" t="s">
+      <c r="H1" s="76" t="s">
         <v>31</v>
       </c>
-      <c r="I1" s="73" t="s">
+      <c r="I1" s="76" t="s">
         <v>32</v>
       </c>
-      <c r="J1" s="73" t="s">
+      <c r="J1" s="76" t="s">
         <v>33</v>
       </c>
-      <c r="K1" s="83" t="s">
+      <c r="K1" s="73" t="s">
         <v>34</v>
       </c>
-      <c r="L1" s="89"/>
-      <c r="M1" s="90"/>
-      <c r="N1" s="80" t="s">
+      <c r="L1" s="84"/>
+      <c r="M1" s="85"/>
+      <c r="N1" s="79" t="s">
         <v>35</v>
       </c>
-      <c r="O1" s="89"/>
-      <c r="P1" s="90"/>
-      <c r="Q1" s="83" t="s">
+      <c r="O1" s="84"/>
+      <c r="P1" s="85"/>
+      <c r="Q1" s="73" t="s">
         <v>8</v>
       </c>
-      <c r="R1" s="89"/>
-      <c r="S1" s="90"/>
-      <c r="T1" s="80" t="s">
+      <c r="R1" s="84"/>
+      <c r="S1" s="85"/>
+      <c r="T1" s="79" t="s">
         <v>9</v>
       </c>
-      <c r="U1" s="89"/>
-      <c r="V1" s="90"/>
-      <c r="W1" s="83" t="s">
+      <c r="U1" s="84"/>
+      <c r="V1" s="85"/>
+      <c r="W1" s="73" t="s">
         <v>10</v>
       </c>
-      <c r="X1" s="89"/>
-      <c r="Y1" s="90"/>
-      <c r="Z1" s="80" t="s">
+      <c r="X1" s="84"/>
+      <c r="Y1" s="85"/>
+      <c r="Z1" s="79" t="s">
         <v>11</v>
       </c>
-      <c r="AA1" s="89"/>
-      <c r="AB1" s="90"/>
-      <c r="AC1" s="83" t="s">
+      <c r="AA1" s="84"/>
+      <c r="AB1" s="85"/>
+      <c r="AC1" s="73" t="s">
         <v>12</v>
       </c>
-      <c r="AD1" s="89"/>
-      <c r="AE1" s="90"/>
-      <c r="AF1" s="80" t="s">
+      <c r="AD1" s="84"/>
+      <c r="AE1" s="85"/>
+      <c r="AF1" s="79" t="s">
         <v>13</v>
       </c>
-      <c r="AG1" s="89"/>
-      <c r="AH1" s="90"/>
-      <c r="AI1" s="83" t="s">
+      <c r="AG1" s="84"/>
+      <c r="AH1" s="85"/>
+      <c r="AI1" s="73" t="s">
         <v>14</v>
       </c>
-      <c r="AJ1" s="89"/>
-      <c r="AK1" s="90"/>
+      <c r="AJ1" s="84"/>
+      <c r="AK1" s="85"/>
       <c r="AL1" s="39"/>
       <c r="AM1" s="66"/>
       <c r="AN1" s="66"/>
@@ -38778,16 +38781,16 @@
       <c r="AS1" s="53"/>
     </row>
     <row r="2" spans="1:45" x14ac:dyDescent="0.2">
-      <c r="A2" s="84"/>
-      <c r="B2" s="87"/>
-      <c r="C2" s="88"/>
-      <c r="D2" s="84"/>
-      <c r="E2" s="84"/>
-      <c r="F2" s="84"/>
-      <c r="G2" s="84"/>
-      <c r="H2" s="84"/>
-      <c r="I2" s="84"/>
-      <c r="J2" s="84"/>
+      <c r="A2" s="86"/>
+      <c r="B2" s="89"/>
+      <c r="C2" s="90"/>
+      <c r="D2" s="86"/>
+      <c r="E2" s="86"/>
+      <c r="F2" s="86"/>
+      <c r="G2" s="86"/>
+      <c r="H2" s="86"/>
+      <c r="I2" s="86"/>
+      <c r="J2" s="86"/>
       <c r="K2" s="3">
         <v>44081</v>
       </c>
@@ -38878,20 +38881,20 @@
       <c r="AS2" s="53"/>
     </row>
     <row r="3" spans="1:45" x14ac:dyDescent="0.2">
-      <c r="A3" s="85"/>
+      <c r="A3" s="87"/>
       <c r="B3" s="8" t="s">
         <v>15</v>
       </c>
       <c r="C3" s="8" t="s">
         <v>16</v>
       </c>
-      <c r="D3" s="85"/>
-      <c r="E3" s="85"/>
-      <c r="F3" s="85"/>
-      <c r="G3" s="85"/>
-      <c r="H3" s="85"/>
-      <c r="I3" s="85"/>
-      <c r="J3" s="85"/>
+      <c r="D3" s="87"/>
+      <c r="E3" s="87"/>
+      <c r="F3" s="87"/>
+      <c r="G3" s="87"/>
+      <c r="H3" s="87"/>
+      <c r="I3" s="87"/>
+      <c r="J3" s="87"/>
       <c r="K3" s="9" t="s">
         <v>36</v>
       </c>
@@ -43881,6 +43884,12 @@
     </row>
   </sheetData>
   <mergeCells count="18">
+    <mergeCell ref="G1:G3"/>
+    <mergeCell ref="A1:A3"/>
+    <mergeCell ref="B1:C2"/>
+    <mergeCell ref="D1:D3"/>
+    <mergeCell ref="E1:E3"/>
+    <mergeCell ref="F1:F3"/>
     <mergeCell ref="AI1:AK1"/>
     <mergeCell ref="H1:H3"/>
     <mergeCell ref="I1:I3"/>
@@ -43893,12 +43902,6 @@
     <mergeCell ref="Z1:AB1"/>
     <mergeCell ref="AC1:AE1"/>
     <mergeCell ref="AF1:AH1"/>
-    <mergeCell ref="G1:G3"/>
-    <mergeCell ref="A1:A3"/>
-    <mergeCell ref="B1:C2"/>
-    <mergeCell ref="D1:D3"/>
-    <mergeCell ref="E1:E3"/>
-    <mergeCell ref="F1:F3"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
@@ -43909,8 +43912,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AK92"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="G4" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="U17" sqref="U17"/>
+    <sheetView tabSelected="1" topLeftCell="A55" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="L90" sqref="L90"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -43920,95 +43923,95 @@
     <col min="3" max="3" width="33" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="61" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="29.5703125" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="24.7109375" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="24.7109375" style="39" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:37" x14ac:dyDescent="0.2">
-      <c r="A1" s="73" t="s">
+      <c r="A1" s="76" t="s">
         <v>26</v>
       </c>
-      <c r="B1" s="76" t="s">
+      <c r="B1" s="80" t="s">
         <v>27</v>
       </c>
-      <c r="C1" s="86"/>
-      <c r="D1" s="73" t="s">
+      <c r="C1" s="88"/>
+      <c r="D1" s="76" t="s">
         <v>28</v>
       </c>
-      <c r="E1" s="73" t="s">
+      <c r="E1" s="76" t="s">
         <v>3</v>
       </c>
-      <c r="F1" s="73" t="s">
+      <c r="F1" s="76" t="s">
         <v>29</v>
       </c>
-      <c r="G1" s="73" t="s">
+      <c r="G1" s="76" t="s">
         <v>30</v>
       </c>
-      <c r="H1" s="73" t="s">
+      <c r="H1" s="76" t="s">
         <v>31</v>
       </c>
-      <c r="I1" s="73" t="s">
+      <c r="I1" s="76" t="s">
         <v>32</v>
       </c>
-      <c r="J1" s="73" t="s">
+      <c r="J1" s="76" t="s">
         <v>33</v>
       </c>
-      <c r="K1" s="83" t="s">
+      <c r="K1" s="73" t="s">
         <v>34</v>
       </c>
-      <c r="L1" s="89"/>
-      <c r="M1" s="90"/>
-      <c r="N1" s="80" t="s">
+      <c r="L1" s="84"/>
+      <c r="M1" s="85"/>
+      <c r="N1" s="79" t="s">
         <v>35</v>
       </c>
-      <c r="O1" s="89"/>
-      <c r="P1" s="90"/>
-      <c r="Q1" s="83" t="s">
+      <c r="O1" s="84"/>
+      <c r="P1" s="85"/>
+      <c r="Q1" s="73" t="s">
         <v>8</v>
       </c>
-      <c r="R1" s="89"/>
-      <c r="S1" s="90"/>
-      <c r="T1" s="80" t="s">
+      <c r="R1" s="84"/>
+      <c r="S1" s="85"/>
+      <c r="T1" s="79" t="s">
         <v>9</v>
       </c>
-      <c r="U1" s="89"/>
-      <c r="V1" s="90"/>
-      <c r="W1" s="83" t="s">
+      <c r="U1" s="84"/>
+      <c r="V1" s="85"/>
+      <c r="W1" s="73" t="s">
         <v>10</v>
       </c>
-      <c r="X1" s="89"/>
-      <c r="Y1" s="90"/>
-      <c r="Z1" s="80" t="s">
+      <c r="X1" s="84"/>
+      <c r="Y1" s="85"/>
+      <c r="Z1" s="79" t="s">
         <v>11</v>
       </c>
-      <c r="AA1" s="89"/>
-      <c r="AB1" s="90"/>
-      <c r="AC1" s="83" t="s">
+      <c r="AA1" s="84"/>
+      <c r="AB1" s="85"/>
+      <c r="AC1" s="73" t="s">
         <v>12</v>
       </c>
-      <c r="AD1" s="89"/>
-      <c r="AE1" s="90"/>
-      <c r="AF1" s="80" t="s">
+      <c r="AD1" s="84"/>
+      <c r="AE1" s="85"/>
+      <c r="AF1" s="79" t="s">
         <v>13</v>
       </c>
-      <c r="AG1" s="89"/>
-      <c r="AH1" s="90"/>
-      <c r="AI1" s="83" t="s">
+      <c r="AG1" s="84"/>
+      <c r="AH1" s="85"/>
+      <c r="AI1" s="73" t="s">
         <v>14</v>
       </c>
-      <c r="AJ1" s="89"/>
-      <c r="AK1" s="90"/>
+      <c r="AJ1" s="84"/>
+      <c r="AK1" s="85"/>
     </row>
     <row r="2" spans="1:37" x14ac:dyDescent="0.2">
-      <c r="A2" s="84"/>
-      <c r="B2" s="87"/>
-      <c r="C2" s="88"/>
-      <c r="D2" s="84"/>
-      <c r="E2" s="84"/>
-      <c r="F2" s="84"/>
-      <c r="G2" s="84"/>
-      <c r="H2" s="84"/>
-      <c r="I2" s="84"/>
-      <c r="J2" s="84"/>
+      <c r="A2" s="86"/>
+      <c r="B2" s="89"/>
+      <c r="C2" s="90"/>
+      <c r="D2" s="86"/>
+      <c r="E2" s="86"/>
+      <c r="F2" s="86"/>
+      <c r="G2" s="86"/>
+      <c r="H2" s="86"/>
+      <c r="I2" s="86"/>
+      <c r="J2" s="86"/>
       <c r="K2" s="3">
         <v>44081</v>
       </c>
@@ -44091,20 +44094,20 @@
       </c>
     </row>
     <row r="3" spans="1:37" x14ac:dyDescent="0.2">
-      <c r="A3" s="85"/>
+      <c r="A3" s="87"/>
       <c r="B3" s="8" t="s">
         <v>15</v>
       </c>
       <c r="C3" s="8" t="s">
         <v>16</v>
       </c>
-      <c r="D3" s="85"/>
-      <c r="E3" s="85"/>
-      <c r="F3" s="85"/>
-      <c r="G3" s="85"/>
-      <c r="H3" s="85"/>
-      <c r="I3" s="85"/>
-      <c r="J3" s="85"/>
+      <c r="D3" s="87"/>
+      <c r="E3" s="87"/>
+      <c r="F3" s="87"/>
+      <c r="G3" s="87"/>
+      <c r="H3" s="87"/>
+      <c r="I3" s="87"/>
+      <c r="J3" s="87"/>
       <c r="K3" s="9" t="s">
         <v>36</v>
       </c>
@@ -44214,10 +44217,7 @@
         <f t="shared" ref="I4" si="0">H4+7</f>
         <v>44088</v>
       </c>
-      <c r="J4" s="39"/>
-      <c r="K4" s="52" t="s">
-        <v>124</v>
-      </c>
+      <c r="K4" s="52"/>
       <c r="L4" s="45"/>
       <c r="M4" s="45"/>
       <c r="N4" s="69"/>
@@ -44263,12 +44263,9 @@
       </c>
       <c r="H5" s="25"/>
       <c r="I5" s="25"/>
-      <c r="J5" s="39"/>
       <c r="K5" s="45"/>
       <c r="L5" s="45"/>
-      <c r="M5" s="45" t="s">
-        <v>153</v>
-      </c>
+      <c r="M5" s="45"/>
       <c r="N5" s="69"/>
       <c r="O5" s="69"/>
       <c r="P5" s="69"/>
@@ -44316,7 +44313,6 @@
       <c r="I6" s="27">
         <v>44081</v>
       </c>
-      <c r="J6" s="39"/>
       <c r="K6" s="45" t="s">
         <v>104</v>
       </c>
@@ -44373,7 +44369,6 @@
       <c r="I7" s="27">
         <v>44081</v>
       </c>
-      <c r="J7" s="39"/>
       <c r="K7" s="45" t="s">
         <v>104</v>
       </c>
@@ -44600,18 +44595,12 @@
       <c r="J11" s="51" t="s">
         <v>101</v>
       </c>
-      <c r="K11" s="45" t="s">
-        <v>117</v>
-      </c>
+      <c r="K11" s="45"/>
       <c r="L11" s="45"/>
-      <c r="M11" s="45" t="s">
-        <v>153</v>
-      </c>
+      <c r="M11" s="45"/>
       <c r="N11" s="69"/>
       <c r="O11" s="69"/>
-      <c r="P11" s="69" t="s">
-        <v>275</v>
-      </c>
+      <c r="P11" s="69"/>
       <c r="Q11" s="45"/>
       <c r="R11" s="45"/>
       <c r="S11" s="45"/>
@@ -44942,9 +44931,7 @@
       </c>
       <c r="K17" s="45"/>
       <c r="L17" s="45"/>
-      <c r="M17" s="45" t="s">
-        <v>134</v>
-      </c>
+      <c r="M17" s="45"/>
       <c r="N17" s="69"/>
       <c r="O17" s="69"/>
       <c r="P17" s="69"/>
@@ -44992,7 +44979,6 @@
       <c r="I18" s="20">
         <v>44085</v>
       </c>
-      <c r="J18" s="39"/>
       <c r="K18" s="45" t="s">
         <v>105</v>
       </c>
@@ -45004,9 +44990,7 @@
       </c>
       <c r="N18" s="69"/>
       <c r="O18" s="69"/>
-      <c r="P18" s="69" t="s">
-        <v>275</v>
-      </c>
+      <c r="P18" s="69"/>
       <c r="Q18" s="45"/>
       <c r="R18" s="45"/>
       <c r="S18" s="45"/>
@@ -45051,7 +45035,6 @@
       <c r="I19" s="20">
         <v>44085</v>
       </c>
-      <c r="J19" s="39"/>
       <c r="K19" s="45" t="s">
         <v>104</v>
       </c>
@@ -45108,7 +45091,6 @@
       <c r="I20" s="20">
         <v>44085</v>
       </c>
-      <c r="J20" s="39"/>
       <c r="K20" s="45" t="s">
         <v>104</v>
       </c>
@@ -45165,7 +45147,6 @@
       <c r="I21" s="20">
         <v>44085</v>
       </c>
-      <c r="J21" s="39"/>
       <c r="K21" s="45" t="s">
         <v>104</v>
       </c>
@@ -45222,7 +45203,6 @@
       <c r="I22" s="20">
         <v>44085</v>
       </c>
-      <c r="J22" s="39"/>
       <c r="K22" s="45" t="s">
         <v>104</v>
       </c>
@@ -45279,11 +45259,8 @@
       <c r="I23" s="20">
         <v>44090</v>
       </c>
-      <c r="J23" s="39"/>
       <c r="K23" s="45"/>
-      <c r="L23" s="45" t="s">
-        <v>19</v>
-      </c>
+      <c r="L23" s="45"/>
       <c r="M23" s="45"/>
       <c r="N23" s="69"/>
       <c r="O23" s="69"/>
@@ -45330,13 +45307,8 @@
       </c>
       <c r="H24" s="25"/>
       <c r="I24" s="25"/>
-      <c r="J24" s="39"/>
-      <c r="K24" s="45">
-        <v>1</v>
-      </c>
-      <c r="L24" s="45" t="s">
-        <v>19</v>
-      </c>
+      <c r="K24" s="45"/>
+      <c r="L24" s="45"/>
       <c r="M24" s="45"/>
       <c r="N24" s="69"/>
       <c r="O24" s="69"/>
@@ -45387,7 +45359,6 @@
       <c r="I25" s="20">
         <v>44086</v>
       </c>
-      <c r="J25" s="39"/>
       <c r="K25" s="45" t="s">
         <v>108</v>
       </c>
@@ -45444,7 +45415,6 @@
       <c r="I26" s="20">
         <v>44087</v>
       </c>
-      <c r="J26" s="39"/>
       <c r="K26" s="45" t="s">
         <v>108</v>
       </c>
@@ -45505,7 +45475,6 @@
       <c r="I27" s="20">
         <v>44087</v>
       </c>
-      <c r="J27" s="39"/>
       <c r="K27" s="45" t="s">
         <v>114</v>
       </c>
@@ -45566,7 +45535,6 @@
       <c r="I28" s="20">
         <v>44087</v>
       </c>
-      <c r="J28" s="39"/>
       <c r="K28" s="45" t="s">
         <v>108</v>
       </c>
@@ -45625,13 +45593,10 @@
       <c r="I29" s="20">
         <v>44089</v>
       </c>
-      <c r="J29" s="39"/>
       <c r="K29" s="45"/>
       <c r="L29" s="45"/>
       <c r="M29" s="45"/>
-      <c r="N29" s="69" t="s">
-        <v>153</v>
-      </c>
+      <c r="N29" s="69"/>
       <c r="O29" s="69"/>
       <c r="P29" s="69"/>
       <c r="Q29" s="45"/>
@@ -45678,7 +45643,6 @@
       <c r="I30" s="20">
         <v>44089</v>
       </c>
-      <c r="J30" s="39"/>
       <c r="K30" s="45"/>
       <c r="L30" s="45"/>
       <c r="M30" s="45"/>
@@ -45735,7 +45699,6 @@
       <c r="I31" s="20">
         <v>44090</v>
       </c>
-      <c r="J31" s="39"/>
       <c r="K31" s="45"/>
       <c r="L31" s="45"/>
       <c r="M31" s="45"/>
@@ -45792,7 +45755,6 @@
       <c r="I32" s="20">
         <v>44090</v>
       </c>
-      <c r="J32" s="39"/>
       <c r="K32" s="45"/>
       <c r="L32" s="45"/>
       <c r="M32" s="45"/>
@@ -45849,13 +45811,10 @@
       <c r="I33" s="20">
         <v>44091</v>
       </c>
-      <c r="J33" s="39"/>
       <c r="K33" s="45"/>
       <c r="L33" s="45"/>
       <c r="M33" s="45"/>
-      <c r="N33" s="69" t="s">
-        <v>160</v>
-      </c>
+      <c r="N33" s="69"/>
       <c r="O33" s="69"/>
       <c r="P33" s="69"/>
       <c r="Q33" s="45"/>
@@ -45902,7 +45861,6 @@
       <c r="I34" s="20">
         <v>44091</v>
       </c>
-      <c r="J34" s="39"/>
       <c r="K34" s="45"/>
       <c r="L34" s="45"/>
       <c r="M34" s="45"/>
@@ -45959,7 +45917,6 @@
       <c r="I35" s="20">
         <v>44091</v>
       </c>
-      <c r="J35" s="39"/>
       <c r="K35" s="45"/>
       <c r="L35" s="45"/>
       <c r="M35" s="45"/>
@@ -46016,7 +45973,6 @@
       <c r="I36" s="20">
         <v>44091</v>
       </c>
-      <c r="J36" s="39"/>
       <c r="K36" s="45"/>
       <c r="L36" s="45"/>
       <c r="M36" s="45"/>
@@ -46055,7 +46011,9 @@
       <c r="A37" s="39">
         <v>32</v>
       </c>
-      <c r="B37" s="39"/>
+      <c r="B37" s="39" t="s">
+        <v>25</v>
+      </c>
       <c r="C37" s="39" t="s">
         <v>154</v>
       </c>
@@ -46073,13 +46031,10 @@
       <c r="I37" s="40">
         <v>44092</v>
       </c>
-      <c r="J37" s="39"/>
       <c r="K37" s="45"/>
       <c r="L37" s="45"/>
       <c r="M37" s="45"/>
-      <c r="N37" s="69" t="s">
-        <v>244</v>
-      </c>
+      <c r="N37" s="69"/>
       <c r="O37" s="69"/>
       <c r="P37" s="69"/>
       <c r="Q37" s="45"/>
@@ -46128,19 +46083,12 @@
       <c r="I38" s="40">
         <v>44092</v>
       </c>
-      <c r="J38" s="39"/>
       <c r="K38" s="45"/>
       <c r="L38" s="45"/>
       <c r="M38" s="45"/>
-      <c r="N38" s="69" t="s">
-        <v>159</v>
-      </c>
-      <c r="O38" s="69" t="s">
-        <v>159</v>
-      </c>
-      <c r="P38" s="69" t="s">
-        <v>134</v>
-      </c>
+      <c r="N38" s="69"/>
+      <c r="O38" s="69"/>
+      <c r="P38" s="69"/>
       <c r="Q38" s="45"/>
       <c r="R38" s="45"/>
       <c r="S38" s="45"/>
@@ -46185,7 +46133,6 @@
       <c r="I39" s="40">
         <v>44092</v>
       </c>
-      <c r="J39" s="39"/>
       <c r="K39" s="45"/>
       <c r="L39" s="45"/>
       <c r="M39" s="45"/>
@@ -46295,17 +46242,12 @@
       </c>
       <c r="H41" s="40"/>
       <c r="I41" s="40"/>
-      <c r="J41" s="39"/>
       <c r="K41" s="45"/>
       <c r="L41" s="45"/>
       <c r="M41" s="45"/>
-      <c r="N41" s="69" t="s">
-        <v>117</v>
-      </c>
+      <c r="N41" s="69"/>
       <c r="O41" s="69"/>
-      <c r="P41" s="69" t="s">
-        <v>276</v>
-      </c>
+      <c r="P41" s="69"/>
       <c r="Q41" s="45"/>
       <c r="R41" s="45"/>
       <c r="S41" s="45"/>
@@ -46350,7 +46292,6 @@
       <c r="I42" s="40">
         <v>44093</v>
       </c>
-      <c r="J42" s="39"/>
       <c r="K42" s="45"/>
       <c r="L42" s="45"/>
       <c r="M42" s="45"/>
@@ -46385,7 +46326,7 @@
       <c r="AJ42" s="45"/>
       <c r="AK42" s="45"/>
     </row>
-    <row r="43" spans="1:37" x14ac:dyDescent="0.2">
+    <row r="43" spans="1:37" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A43" s="39">
         <v>37</v>
       </c>
@@ -46407,7 +46348,6 @@
       <c r="I43" s="40">
         <v>44093</v>
       </c>
-      <c r="J43" s="39"/>
       <c r="K43" s="45"/>
       <c r="L43" s="45"/>
       <c r="M43" s="45"/>
@@ -46464,16 +46404,13 @@
       <c r="I44" s="35">
         <v>44095</v>
       </c>
-      <c r="J44" s="39"/>
       <c r="K44" s="45"/>
       <c r="L44" s="45"/>
       <c r="M44" s="45"/>
       <c r="N44" s="69"/>
       <c r="O44" s="69"/>
       <c r="P44" s="69"/>
-      <c r="Q44" s="45" t="s">
-        <v>269</v>
-      </c>
+      <c r="Q44" s="45"/>
       <c r="R44" s="45"/>
       <c r="S44" s="45"/>
       <c r="T44" s="69"/>
@@ -46519,16 +46456,13 @@
       <c r="I45" s="35">
         <v>44095</v>
       </c>
-      <c r="J45" s="39"/>
       <c r="K45" s="45"/>
       <c r="L45" s="45"/>
       <c r="M45" s="45"/>
       <c r="N45" s="69"/>
       <c r="O45" s="69"/>
       <c r="P45" s="69"/>
-      <c r="Q45" s="45" t="s">
-        <v>269</v>
-      </c>
+      <c r="Q45" s="45"/>
       <c r="R45" s="45"/>
       <c r="S45" s="45"/>
       <c r="T45" s="69"/>
@@ -46572,7 +46506,6 @@
       <c r="I46" s="35">
         <v>44095</v>
       </c>
-      <c r="J46" s="39"/>
       <c r="K46" s="45"/>
       <c r="L46" s="45"/>
       <c r="M46" s="45"/>
@@ -46629,7 +46562,6 @@
       <c r="I47" s="35">
         <v>44095</v>
       </c>
-      <c r="J47" s="39"/>
       <c r="K47" s="45"/>
       <c r="L47" s="45"/>
       <c r="M47" s="45"/>
@@ -46686,7 +46618,6 @@
       <c r="I48" s="35">
         <v>44096</v>
       </c>
-      <c r="J48" s="39"/>
       <c r="K48" s="45"/>
       <c r="L48" s="45"/>
       <c r="M48" s="45"/>
@@ -46739,16 +46670,13 @@
       <c r="I49" s="40">
         <v>44097</v>
       </c>
-      <c r="J49" s="39"/>
       <c r="K49" s="45"/>
       <c r="L49" s="45"/>
       <c r="M49" s="45"/>
       <c r="N49" s="69"/>
       <c r="O49" s="69"/>
       <c r="P49" s="69"/>
-      <c r="Q49" s="45" t="s">
-        <v>159</v>
-      </c>
+      <c r="Q49" s="45"/>
       <c r="R49" s="45"/>
       <c r="S49" s="45"/>
       <c r="T49" s="69"/>
@@ -46794,16 +46722,13 @@
       <c r="I50" s="40">
         <v>44097</v>
       </c>
-      <c r="J50" s="39"/>
       <c r="K50" s="45"/>
       <c r="L50" s="45"/>
       <c r="M50" s="45"/>
       <c r="N50" s="69"/>
       <c r="O50" s="69"/>
       <c r="P50" s="69"/>
-      <c r="Q50" s="45" t="s">
-        <v>159</v>
-      </c>
+      <c r="Q50" s="45"/>
       <c r="R50" s="45"/>
       <c r="S50" s="45"/>
       <c r="T50" s="69"/>
@@ -46847,7 +46772,6 @@
       <c r="I51" s="40">
         <v>44097</v>
       </c>
-      <c r="J51" s="39"/>
       <c r="K51" s="45"/>
       <c r="L51" s="45"/>
       <c r="M51" s="45"/>
@@ -46900,7 +46824,6 @@
       <c r="I52" s="40">
         <v>44097</v>
       </c>
-      <c r="J52" s="39"/>
       <c r="K52" s="45"/>
       <c r="L52" s="45"/>
       <c r="M52" s="45"/>
@@ -46955,16 +46878,13 @@
       <c r="I53" s="40">
         <v>44100</v>
       </c>
-      <c r="J53" s="39"/>
       <c r="K53" s="45"/>
       <c r="L53" s="45"/>
       <c r="M53" s="45"/>
       <c r="N53" s="69"/>
       <c r="O53" s="69"/>
       <c r="P53" s="69"/>
-      <c r="Q53" s="45" t="s">
-        <v>164</v>
-      </c>
+      <c r="Q53" s="45"/>
       <c r="R53" s="45"/>
       <c r="S53" s="45"/>
       <c r="T53" s="69"/>
@@ -47010,16 +46930,13 @@
       <c r="I54" s="40">
         <v>44098</v>
       </c>
-      <c r="J54" s="39"/>
       <c r="K54" s="45"/>
       <c r="L54" s="45"/>
       <c r="M54" s="45"/>
       <c r="N54" s="69"/>
       <c r="O54" s="69"/>
       <c r="P54" s="69"/>
-      <c r="Q54" s="45" t="s">
-        <v>158</v>
-      </c>
+      <c r="Q54" s="45"/>
       <c r="R54" s="45"/>
       <c r="S54" s="45"/>
       <c r="T54" s="69"/>
@@ -47063,7 +46980,6 @@
       <c r="I55" s="40">
         <v>44098</v>
       </c>
-      <c r="J55" s="39"/>
       <c r="K55" s="45"/>
       <c r="L55" s="45"/>
       <c r="M55" s="45"/>
@@ -47120,7 +47036,6 @@
       <c r="I56" s="40">
         <v>44098</v>
       </c>
-      <c r="J56" s="39"/>
       <c r="K56" s="45"/>
       <c r="L56" s="45"/>
       <c r="M56" s="45"/>
@@ -47177,7 +47092,6 @@
       <c r="I57" s="40">
         <v>44098</v>
       </c>
-      <c r="J57" s="39"/>
       <c r="K57" s="45"/>
       <c r="L57" s="45"/>
       <c r="M57" s="45"/>
@@ -47234,7 +47148,6 @@
       <c r="I58" s="40">
         <v>44098</v>
       </c>
-      <c r="J58" s="39"/>
       <c r="K58" s="45"/>
       <c r="L58" s="45"/>
       <c r="M58" s="45"/>
@@ -47293,16 +47206,13 @@
       <c r="I59" s="40">
         <v>44100</v>
       </c>
-      <c r="J59" s="39"/>
       <c r="K59" s="45"/>
       <c r="L59" s="45"/>
       <c r="M59" s="45"/>
       <c r="N59" s="69"/>
       <c r="O59" s="69"/>
       <c r="P59" s="69"/>
-      <c r="Q59" s="45" t="s">
-        <v>159</v>
-      </c>
+      <c r="Q59" s="45"/>
       <c r="R59" s="45"/>
       <c r="S59" s="45"/>
       <c r="T59" s="69"/>
@@ -47346,7 +47256,6 @@
       <c r="I60" s="40">
         <v>44100</v>
       </c>
-      <c r="J60" s="39"/>
       <c r="K60" s="45"/>
       <c r="L60" s="45"/>
       <c r="M60" s="45"/>
@@ -47356,7 +47265,9 @@
       <c r="Q60" s="45" t="s">
         <v>156</v>
       </c>
-      <c r="R60" s="45"/>
+      <c r="R60" s="45" t="s">
+        <v>156</v>
+      </c>
       <c r="S60" s="45" t="s">
         <v>153</v>
       </c>
@@ -47401,7 +47312,6 @@
       <c r="I61" s="40">
         <v>44100</v>
       </c>
-      <c r="J61" s="39"/>
       <c r="K61" s="45"/>
       <c r="L61" s="45"/>
       <c r="M61" s="45"/>
@@ -47456,16 +47366,13 @@
       <c r="I62" s="40">
         <v>44099</v>
       </c>
-      <c r="J62" s="39"/>
       <c r="K62" s="45"/>
       <c r="L62" s="45"/>
       <c r="M62" s="45"/>
       <c r="N62" s="69"/>
       <c r="O62" s="69"/>
       <c r="P62" s="69"/>
-      <c r="Q62" s="45" t="s">
-        <v>271</v>
-      </c>
+      <c r="Q62" s="45"/>
       <c r="R62" s="45"/>
       <c r="S62" s="45"/>
       <c r="T62" s="69"/>
@@ -47511,16 +47418,13 @@
       <c r="I63" s="40">
         <v>44099</v>
       </c>
-      <c r="J63" s="39"/>
       <c r="K63" s="45"/>
       <c r="L63" s="45"/>
       <c r="M63" s="45"/>
       <c r="N63" s="69"/>
       <c r="O63" s="69"/>
       <c r="P63" s="69"/>
-      <c r="Q63" s="45" t="s">
-        <v>159</v>
-      </c>
+      <c r="Q63" s="45"/>
       <c r="R63" s="45"/>
       <c r="S63" s="45"/>
       <c r="T63" s="69"/>
@@ -47564,7 +47468,6 @@
       <c r="I64" s="40">
         <v>44099</v>
       </c>
-      <c r="J64" s="39"/>
       <c r="K64" s="45"/>
       <c r="L64" s="45"/>
       <c r="M64" s="45"/>
@@ -47617,7 +47520,6 @@
       <c r="I65" s="40">
         <v>44099</v>
       </c>
-      <c r="J65" s="39"/>
       <c r="K65" s="45"/>
       <c r="L65" s="45"/>
       <c r="M65" s="45"/>
@@ -47674,7 +47576,6 @@
       <c r="I66" s="40">
         <v>44099</v>
       </c>
-      <c r="J66" s="39"/>
       <c r="K66" s="45"/>
       <c r="L66" s="45"/>
       <c r="M66" s="45"/>
@@ -47729,16 +47630,13 @@
       <c r="I67" s="40">
         <v>44099</v>
       </c>
-      <c r="J67" s="39"/>
       <c r="K67" s="45"/>
       <c r="L67" s="45"/>
       <c r="M67" s="45"/>
       <c r="N67" s="69"/>
       <c r="O67" s="69"/>
       <c r="P67" s="69"/>
-      <c r="Q67" s="45" t="s">
-        <v>156</v>
-      </c>
+      <c r="Q67" s="45"/>
       <c r="R67" s="45"/>
       <c r="S67" s="45"/>
       <c r="T67" s="69"/>
@@ -47782,7 +47680,6 @@
       <c r="I68" s="40">
         <v>44099</v>
       </c>
-      <c r="J68" s="39"/>
       <c r="K68" s="45"/>
       <c r="L68" s="45"/>
       <c r="M68" s="45"/>
@@ -47835,7 +47732,6 @@
       <c r="I69" s="40">
         <v>44099</v>
       </c>
-      <c r="J69" s="39"/>
       <c r="K69" s="45"/>
       <c r="L69" s="45"/>
       <c r="M69" s="45"/>
@@ -47890,16 +47786,13 @@
       <c r="I70" s="40">
         <v>44099</v>
       </c>
-      <c r="J70" s="39"/>
       <c r="K70" s="45"/>
       <c r="L70" s="45"/>
       <c r="M70" s="45"/>
       <c r="N70" s="69"/>
       <c r="O70" s="69"/>
       <c r="P70" s="69"/>
-      <c r="Q70" s="45" t="s">
-        <v>163</v>
-      </c>
+      <c r="Q70" s="45"/>
       <c r="R70" s="45"/>
       <c r="S70" s="45"/>
       <c r="T70" s="69"/>
@@ -47943,7 +47836,6 @@
       <c r="I71" s="40">
         <v>44099</v>
       </c>
-      <c r="J71" s="39"/>
       <c r="K71" s="45"/>
       <c r="L71" s="45"/>
       <c r="M71" s="45"/>
@@ -48000,7 +47892,6 @@
       <c r="I72" s="40">
         <v>44099</v>
       </c>
-      <c r="J72" s="39"/>
       <c r="K72" s="45"/>
       <c r="L72" s="45"/>
       <c r="M72" s="45"/>
@@ -48057,7 +47948,6 @@
       <c r="I73" s="40">
         <v>44099</v>
       </c>
-      <c r="J73" s="39"/>
       <c r="K73" s="45"/>
       <c r="L73" s="45"/>
       <c r="M73" s="45"/>
@@ -48114,7 +48004,6 @@
       <c r="I74" s="40">
         <v>44099</v>
       </c>
-      <c r="J74" s="39"/>
       <c r="K74" s="45"/>
       <c r="L74" s="45"/>
       <c r="M74" s="45"/>
@@ -48182,9 +48071,7 @@
       <c r="Q75" s="45"/>
       <c r="R75" s="45"/>
       <c r="S75" s="45"/>
-      <c r="T75" s="69" t="s">
-        <v>156</v>
-      </c>
+      <c r="T75" s="69"/>
       <c r="U75" s="69"/>
       <c r="V75" s="69"/>
       <c r="W75" s="45"/>
@@ -48234,9 +48121,7 @@
       <c r="Q76" s="45"/>
       <c r="R76" s="45"/>
       <c r="S76" s="45"/>
-      <c r="T76" s="69" t="s">
-        <v>156</v>
-      </c>
+      <c r="T76" s="69"/>
       <c r="U76" s="69"/>
       <c r="V76" s="69"/>
       <c r="W76" s="45"/>
@@ -48383,6 +48268,7 @@
       <c r="I79" s="70">
         <v>44103</v>
       </c>
+      <c r="J79" s="39"/>
       <c r="K79" s="45"/>
       <c r="L79" s="45"/>
       <c r="M79" s="45"/>
@@ -48392,9 +48278,7 @@
       <c r="Q79" s="45"/>
       <c r="R79" s="45"/>
       <c r="S79" s="45"/>
-      <c r="T79" s="69" t="s">
-        <v>290</v>
-      </c>
+      <c r="T79" s="69"/>
       <c r="U79" s="69"/>
       <c r="V79" s="69"/>
       <c r="W79" s="45"/>
@@ -48437,7 +48321,7 @@
       <c r="I80" s="70">
         <v>44103</v>
       </c>
-      <c r="J80" t="s">
+      <c r="J80" s="39" t="s">
         <v>291</v>
       </c>
       <c r="K80" s="45"/>
@@ -48449,9 +48333,7 @@
       <c r="Q80" s="45"/>
       <c r="R80" s="45"/>
       <c r="S80" s="45"/>
-      <c r="T80" s="69" t="s">
-        <v>289</v>
-      </c>
+      <c r="T80" s="69"/>
       <c r="U80" s="69"/>
       <c r="V80" s="69"/>
       <c r="W80" s="45"/>
@@ -48659,9 +48541,7 @@
       <c r="Q84" s="45"/>
       <c r="R84" s="45"/>
       <c r="S84" s="45"/>
-      <c r="T84" s="69" t="s">
-        <v>289</v>
-      </c>
+      <c r="T84" s="69"/>
       <c r="U84" s="69"/>
       <c r="V84" s="69"/>
       <c r="W84" s="45"/>
@@ -48860,6 +48740,9 @@
       <c r="I88" s="70">
         <v>44105</v>
       </c>
+      <c r="J88" s="39" t="s">
+        <v>292</v>
+      </c>
       <c r="K88" s="45"/>
       <c r="L88" s="45"/>
       <c r="M88" s="45"/>
@@ -48869,9 +48752,7 @@
       <c r="Q88" s="45"/>
       <c r="R88" s="45"/>
       <c r="S88" s="45"/>
-      <c r="T88" s="69" t="s">
-        <v>277</v>
-      </c>
+      <c r="T88" s="69"/>
       <c r="U88" s="69"/>
       <c r="V88" s="69"/>
       <c r="W88" s="45"/>
@@ -49012,12 +48893,6 @@
     </row>
   </sheetData>
   <mergeCells count="18">
-    <mergeCell ref="G1:G3"/>
-    <mergeCell ref="A1:A3"/>
-    <mergeCell ref="B1:C2"/>
-    <mergeCell ref="D1:D3"/>
-    <mergeCell ref="E1:E3"/>
-    <mergeCell ref="F1:F3"/>
     <mergeCell ref="AI1:AK1"/>
     <mergeCell ref="H1:H3"/>
     <mergeCell ref="I1:I3"/>
@@ -49030,6 +48905,12 @@
     <mergeCell ref="Z1:AB1"/>
     <mergeCell ref="AC1:AE1"/>
     <mergeCell ref="AF1:AH1"/>
+    <mergeCell ref="G1:G3"/>
+    <mergeCell ref="A1:A3"/>
+    <mergeCell ref="B1:C2"/>
+    <mergeCell ref="D1:D3"/>
+    <mergeCell ref="E1:E3"/>
+    <mergeCell ref="F1:F3"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>